<commit_message>
Add Ant Colony Optimization (ACO) for continuous domain to swarm-based
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="606" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="614" uniqueCount="186">
   <si>
     <t>Group</t>
   </si>
@@ -571,6 +571,12 @@
   </si>
   <si>
     <t>BRO</t>
+  </si>
+  <si>
+    <t>Ant Colony Optimization</t>
+  </si>
+  <si>
+    <t>ACO</t>
   </si>
 </sst>
 </file>
@@ -1469,10 +1475,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M85"/>
+  <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="O71" sqref="O71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1924,13 +1930,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>43</v>
+        <v>184</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>44</v>
+        <v>185</v>
       </c>
       <c r="E14" s="2">
-        <v>2010</v>
+        <v>2008</v>
       </c>
       <c r="F14" s="2" t="s">
         <v>12</v>
@@ -1948,7 +1954,7 @@
         <v>13</v>
       </c>
       <c r="K14" s="2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="L14" s="2" t="s">
         <v>31</v>
@@ -1956,13 +1962,13 @@
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="E15" s="2">
         <v>2010</v>
@@ -1971,54 +1977,54 @@
         <v>12</v>
       </c>
       <c r="G15" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K15" s="2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>176</v>
+        <v>45</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>177</v>
+        <v>46</v>
       </c>
       <c r="E16" s="2">
-        <v>2012</v>
+        <v>2010</v>
       </c>
       <c r="F16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G16" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>178</v>
+        <v>20</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K16" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>15</v>
@@ -2026,19 +2032,19 @@
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>47</v>
+        <v>176</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>48</v>
+        <v>177</v>
       </c>
       <c r="E17" s="2">
-        <v>2013</v>
+        <v>2012</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>13</v>
@@ -2047,33 +2053,33 @@
         <v>13</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>20</v>
+        <v>178</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K17" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="E18" s="2">
-        <v>2014</v>
+        <v>2013</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>13</v>
@@ -2082,48 +2088,48 @@
         <v>13</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K18" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="2">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E19" s="2">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="F19" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G19" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H19" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K19" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L19" s="2" t="s">
         <v>15</v>
@@ -2131,13 +2137,13 @@
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E20" s="2">
         <v>2015</v>
@@ -2146,39 +2152,39 @@
         <v>12</v>
       </c>
       <c r="G20" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H20" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K20" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="2">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E21" s="2">
         <v>2015</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>13</v>
@@ -2190,30 +2196,30 @@
         <v>14</v>
       </c>
       <c r="J21" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K21" s="2">
         <v>2</v>
       </c>
       <c r="L21" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="2">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>171</v>
+        <v>58</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E22" s="2">
         <v>2015</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>13</v>
@@ -2222,13 +2228,13 @@
         <v>13</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K22" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L22" s="2" t="s">
         <v>15</v>
@@ -2236,19 +2242,19 @@
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="2">
-        <v>14</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>179</v>
+        <v>13</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>171</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>180</v>
+        <v>60</v>
       </c>
       <c r="E23" s="2">
-        <v>2016</v>
+        <v>2015</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>181</v>
+        <v>12</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>13</v>
@@ -2257,13 +2263,13 @@
         <v>13</v>
       </c>
       <c r="I23" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J23" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K23" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>15</v>
@@ -2271,28 +2277,28 @@
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="2">
-        <v>15</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>61</v>
+        <v>14</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>179</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>62</v>
+        <v>180</v>
       </c>
       <c r="E24" s="2">
         <v>2016</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>12</v>
+        <v>181</v>
       </c>
       <c r="G24" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="J24" s="2" t="s">
         <v>28</v>
@@ -2306,13 +2312,13 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="2">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="E25" s="2">
         <v>2016</v>
@@ -2321,39 +2327,39 @@
         <v>12</v>
       </c>
       <c r="G25" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H25" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="J25" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K25" s="2">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="26" spans="2:12">
       <c r="B26" s="2">
-        <v>17</v>
-      </c>
-      <c r="C26" s="3" t="s">
-        <v>172</v>
+        <v>16</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>64</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>173</v>
+        <v>65</v>
       </c>
       <c r="E26" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>13</v>
@@ -2362,13 +2368,13 @@
         <v>13</v>
       </c>
       <c r="I26" s="2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J26" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K26" s="2">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="L26" s="2" t="s">
         <v>31</v>
@@ -2376,19 +2382,19 @@
     </row>
     <row r="27" spans="2:12">
       <c r="B27" s="2">
-        <v>18</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>66</v>
+        <v>17</v>
+      </c>
+      <c r="C27" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>67</v>
+        <v>173</v>
       </c>
       <c r="E27" s="2">
         <v>2017</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>13</v>
@@ -2397,27 +2403,27 @@
         <v>13</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K27" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>49</v>
+        <v>31</v>
       </c>
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="2">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E28" s="2">
         <v>2017</v>
@@ -2426,54 +2432,54 @@
         <v>12</v>
       </c>
       <c r="G28" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H28" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K28" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="2">
+        <v>19</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2017</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I29" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E29" s="2">
-        <v>2018</v>
-      </c>
-      <c r="F29" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G29" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H29" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="I29" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="J29" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K29" s="2">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L29" s="2" t="s">
         <v>15</v>
@@ -2481,34 +2487,34 @@
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="2">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E30" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G30" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I30" s="2" t="s">
         <v>14</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K30" s="2">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="L30" s="2" t="s">
         <v>15</v>
@@ -2516,22 +2522,22 @@
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="2">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E31" s="2">
         <v>2019</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G31" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H31" s="2" t="s">
         <v>13</v>
@@ -2540,59 +2546,59 @@
         <v>14</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K31" s="2">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="2">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E32" s="2">
         <v>2019</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G32" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K32" s="2">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="33" spans="1:12">
       <c r="B33" s="2">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E33" s="2">
         <v>2019</v>
@@ -2601,33 +2607,33 @@
         <v>12</v>
       </c>
       <c r="G33" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K33" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L33" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="34" spans="1:12">
       <c r="B34" s="2">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E34" s="2">
         <v>2019</v>
@@ -2636,19 +2642,19 @@
         <v>12</v>
       </c>
       <c r="G34" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>63</v>
+        <v>94</v>
       </c>
       <c r="J34" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K34" s="2">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L34" s="2" t="s">
         <v>31</v>
@@ -2656,25 +2662,25 @@
     </row>
     <row r="35" spans="1:12">
       <c r="B35" s="2">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E35" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>12</v>
       </c>
       <c r="G35" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I35" s="2" t="s">
         <v>63</v>
@@ -2683,21 +2689,21 @@
         <v>28</v>
       </c>
       <c r="K35" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:12">
       <c r="B36" s="2">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E36" s="2">
         <v>2020</v>
@@ -2712,86 +2718,86 @@
         <v>13</v>
       </c>
       <c r="I36" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K36" s="2">
+        <v>3</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="B37" s="2">
+        <v>27</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="E37" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I37" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J36" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K36" s="2">
+      <c r="J37" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K37" s="2">
         <v>5</v>
       </c>
-      <c r="L36" s="2" t="s">
+      <c r="L37" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="1:12">
-      <c r="A39" s="2" t="s">
+    <row r="40" spans="1:12">
+      <c r="A40" s="2" t="s">
         <v>169</v>
       </c>
-      <c r="B39" s="2">
+      <c r="B40" s="2">
         <v>1</v>
       </c>
-      <c r="C39" s="2" t="s">
+      <c r="C40" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="D39" s="2" t="s">
+      <c r="D40" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="E39" s="2">
+      <c r="E40" s="2">
         <v>2013</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I39" s="2" t="s">
+      <c r="F40" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I40" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J39" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K39" s="2">
+      <c r="J40" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K40" s="2">
         <v>7</v>
-      </c>
-      <c r="L39" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12">
-      <c r="B40" s="2">
-        <v>2</v>
-      </c>
-      <c r="C40" s="2" t="s">
-        <v>97</v>
-      </c>
-      <c r="D40" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E40" s="2">
-        <v>2016</v>
-      </c>
-      <c r="F40" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G40" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="2">
-        <v>3</v>
       </c>
       <c r="L40" s="2" t="s">
         <v>15</v>
@@ -2799,34 +2805,34 @@
     </row>
     <row r="41" spans="1:12">
       <c r="B41" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E41" s="2">
         <v>2016</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="G41" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J41" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K41" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L41" s="2" t="s">
         <v>15</v>
@@ -2834,22 +2840,22 @@
     </row>
     <row r="42" spans="1:12">
       <c r="B42" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E42" s="2">
         <v>2016</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="G42" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H42" s="2" t="s">
         <v>13</v>
@@ -2858,10 +2864,10 @@
         <v>14</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K42" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L42" s="2" t="s">
         <v>15</v>
@@ -2869,60 +2875,60 @@
     </row>
     <row r="43" spans="1:12">
       <c r="B43" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C43" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D43" s="2" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E43" s="2">
-        <v>2019</v>
+        <v>2016</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>101</v>
+        <v>12</v>
       </c>
       <c r="G43" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>28</v>
       </c>
       <c r="K43" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="44" spans="1:12">
       <c r="B44" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D44" s="2" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E44" s="2">
         <v>2019</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>12</v>
+        <v>101</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>13</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>63</v>
@@ -2931,21 +2937,21 @@
         <v>28</v>
       </c>
       <c r="K44" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:12">
       <c r="B45" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C45" s="2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="D45" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E45" s="2">
         <v>2019</v>
@@ -2960,13 +2966,13 @@
         <v>13</v>
       </c>
       <c r="I45" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J45" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K45" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L45" s="2" t="s">
         <v>31</v>
@@ -2974,13 +2980,13 @@
     </row>
     <row r="46" spans="1:12">
       <c r="B46" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="D46" s="2" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E46" s="2">
         <v>2019</v>
@@ -2995,65 +3001,65 @@
         <v>13</v>
       </c>
       <c r="I46" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K46" s="2">
+        <v>4</v>
+      </c>
+      <c r="L46" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="B47" s="2">
+        <v>8</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="E47" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H47" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I47" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="J46" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K46" s="2">
+      <c r="J47" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K47" s="2">
         <v>2</v>
       </c>
-      <c r="L46" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="A48" s="2" t="s">
+      <c r="L47" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="B48" s="2">
+      <c r="B49" s="2">
         <v>1</v>
       </c>
-      <c r="C48" s="2" t="s">
+      <c r="C49" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="D48" s="2" t="s">
+      <c r="D49" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="E48" s="2">
-        <v>2011</v>
-      </c>
-      <c r="F48" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="J48" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="2">
-        <v>2</v>
-      </c>
-      <c r="L48" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12">
-      <c r="B49" s="2">
-        <v>2</v>
-      </c>
-      <c r="C49" s="2" t="s">
-        <v>115</v>
-      </c>
-      <c r="D49" s="2" t="s">
-        <v>116</v>
       </c>
       <c r="E49" s="2">
         <v>2011</v>
@@ -3062,39 +3068,39 @@
         <v>12</v>
       </c>
       <c r="G49" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I49" s="2" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K49" s="2">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="50" spans="1:12">
       <c r="B50" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C50" s="2" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D50" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E50" s="2">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>13</v>
@@ -3103,36 +3109,36 @@
         <v>13</v>
       </c>
       <c r="I50" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J50" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K50" s="2">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L50" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="51" spans="1:12">
       <c r="B51" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C51" s="2" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D51" s="2" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E51" s="2">
         <v>2019</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G51" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H51" s="2" t="s">
         <v>13</v>
@@ -3144,21 +3150,21 @@
         <v>28</v>
       </c>
       <c r="K51" s="2">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L51" s="2" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:12">
       <c r="B52" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C52" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D52" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E52" s="2">
         <v>2019</v>
@@ -3179,21 +3185,21 @@
         <v>28</v>
       </c>
       <c r="K52" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L52" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="B53" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C53" s="2" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D53" s="2" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E53" s="2">
         <v>2019</v>
@@ -3202,13 +3208,13 @@
         <v>12</v>
       </c>
       <c r="G53" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H53" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I53" s="2" t="s">
-        <v>94</v>
+        <v>14</v>
       </c>
       <c r="J53" s="2" t="s">
         <v>28</v>
@@ -3222,13 +3228,13 @@
     </row>
     <row r="54" spans="1:12">
       <c r="B54" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C54" s="2" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D54" s="2" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E54" s="2">
         <v>2019</v>
@@ -3243,13 +3249,13 @@
         <v>13</v>
       </c>
       <c r="I54" s="2" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="J54" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K54" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L54" s="2" t="s">
         <v>15</v>
@@ -3257,19 +3263,19 @@
     </row>
     <row r="55" spans="1:12">
       <c r="B55" s="2">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C55" s="2" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D55" s="2" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="E55" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>13</v>
@@ -3278,33 +3284,33 @@
         <v>13</v>
       </c>
       <c r="I55" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J55" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K55" s="2">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L55" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="B56" s="2">
-        <v>9</v>
-      </c>
-      <c r="C56" s="3" t="s">
-        <v>174</v>
+        <v>8</v>
+      </c>
+      <c r="C56" s="2" t="s">
+        <v>127</v>
       </c>
       <c r="D56" s="2" t="s">
-        <v>175</v>
+        <v>128</v>
       </c>
       <c r="E56" s="2">
         <v>2020</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>13</v>
@@ -3313,71 +3319,71 @@
         <v>13</v>
       </c>
       <c r="I56" s="2" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J56" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K56" s="2">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L56" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="58" spans="1:12">
-      <c r="A58" s="2" t="s">
+    <row r="57" spans="1:12">
+      <c r="B57" s="2">
+        <v>9</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="D57" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E57" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="2">
+        <v>2</v>
+      </c>
+      <c r="L57" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B58" s="2">
+      <c r="B59" s="2">
         <v>1</v>
       </c>
-      <c r="C58" s="2" t="s">
+      <c r="C59" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="D58" s="2" t="s">
+      <c r="D59" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="E58" s="2">
+      <c r="E59" s="2">
         <v>2006</v>
       </c>
-      <c r="F58" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K58" s="2">
-        <v>5</v>
-      </c>
-      <c r="L58" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="B59" s="2">
-        <v>2</v>
-      </c>
-      <c r="C59" s="2" t="s">
-        <v>132</v>
-      </c>
-      <c r="D59" s="2" t="s">
-        <v>133</v>
-      </c>
-      <c r="E59" s="2">
-        <v>2008</v>
-      </c>
       <c r="F59" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>13</v>
@@ -3392,7 +3398,7 @@
         <v>28</v>
       </c>
       <c r="K59" s="2">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L59" s="2" t="s">
         <v>15</v>
@@ -3400,51 +3406,51 @@
     </row>
     <row r="60" spans="1:12">
       <c r="B60" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C60" s="2" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D60" s="2" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E60" s="2">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="F60" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G60" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H60" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="2" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J60" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K60" s="2">
         <v>4</v>
       </c>
       <c r="L60" s="2" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="B61" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="2" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D61" s="2" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E61" s="2">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F61" s="2" t="s">
         <v>42</v>
@@ -3456,36 +3462,36 @@
         <v>13</v>
       </c>
       <c r="I61" s="2" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J61" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K61" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L61" s="2" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="B62" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" s="2" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="D62" s="2" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="E62" s="2">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F62" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G62" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H62" s="2" t="s">
         <v>13</v>
@@ -3497,24 +3503,24 @@
         <v>28</v>
       </c>
       <c r="K62" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L62" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="B63" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" s="2" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D63" s="2" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="E63" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F63" s="2" t="s">
         <v>42</v>
@@ -3532,7 +3538,7 @@
         <v>28</v>
       </c>
       <c r="K63" s="2">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L63" s="2" t="s">
         <v>31</v>
@@ -3540,22 +3546,22 @@
     </row>
     <row r="64" spans="1:12">
       <c r="B64" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" s="2" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D64" s="2" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E64" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F64" s="2" t="s">
         <v>42</v>
       </c>
       <c r="G64" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H64" s="2" t="s">
         <v>13</v>
@@ -3567,62 +3573,62 @@
         <v>28</v>
       </c>
       <c r="K64" s="2">
+        <v>12</v>
+      </c>
+      <c r="L64" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="65" spans="1:12">
+      <c r="B65" s="2">
+        <v>7</v>
+      </c>
+      <c r="C65" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D65" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E65" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F65" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H65" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J65" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K65" s="2">
         <v>3</v>
       </c>
-      <c r="L64" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12">
-      <c r="A66" s="2" t="s">
+      <c r="L65" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12">
+      <c r="A67" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B66" s="2">
+      <c r="B67" s="2">
         <v>1</v>
       </c>
-      <c r="C66" s="2" t="s">
+      <c r="C67" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D66" s="2" t="s">
+      <c r="D67" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E66" s="2">
+      <c r="E67" s="2">
         <v>2018</v>
-      </c>
-      <c r="F66" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K66" s="2">
-        <v>4</v>
-      </c>
-      <c r="L66" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12">
-      <c r="B67" s="2">
-        <v>2</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>147</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>148</v>
-      </c>
-      <c r="E67" s="2">
-        <v>2019</v>
       </c>
       <c r="F67" s="2" t="s">
         <v>42</v>
@@ -3634,182 +3640,182 @@
         <v>13</v>
       </c>
       <c r="I67" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J67" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K67" s="2">
+        <v>4</v>
+      </c>
+      <c r="L67" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="68" spans="1:12">
+      <c r="B68" s="2">
+        <v>2</v>
+      </c>
+      <c r="C68" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E68" s="2">
+        <v>2019</v>
+      </c>
+      <c r="F68" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="G68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H68" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I68" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="J67" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="K67" s="2">
+      <c r="J68" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K68" s="2">
         <v>2</v>
       </c>
-      <c r="L67" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="69" spans="1:12">
-      <c r="A69" s="2" t="s">
+      <c r="L68" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="70" spans="1:12">
+      <c r="A70" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="B69" s="2">
+      <c r="B70" s="2">
         <v>1</v>
       </c>
-      <c r="C69" s="2" t="s">
+      <c r="C70" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="D69" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>151</v>
       </c>
-      <c r="E69" s="2">
+      <c r="E70" s="2">
         <v>2016</v>
       </c>
-      <c r="F69" s="2" t="s">
+      <c r="F70" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G69" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I69" s="2" t="s">
+      <c r="G70" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J69" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K69" s="2">
+      <c r="J70" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K70" s="2">
         <v>2</v>
       </c>
-      <c r="L69" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="A71" s="2" t="s">
+      <c r="L70" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B71" s="2">
+      <c r="B72" s="2">
         <v>1</v>
       </c>
-      <c r="C71" s="2" t="s">
+      <c r="C72" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="2" t="s">
+      <c r="D72" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E71" s="2">
+      <c r="E72" s="2">
         <v>2001</v>
       </c>
-      <c r="F71" s="2" t="s">
+      <c r="F72" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="G71" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I71" s="2" t="s">
+      <c r="G72" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I72" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J71" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K71" s="2">
+      <c r="J72" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K72" s="2">
         <v>5</v>
       </c>
-      <c r="L71" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12">
-      <c r="A73" s="2" t="s">
+      <c r="L72" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12">
+      <c r="A74" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="B73" s="2">
+      <c r="B74" s="2">
         <v>1</v>
       </c>
-      <c r="C73" s="5" t="s">
+      <c r="C74" s="5" t="s">
         <v>155</v>
       </c>
-      <c r="D73" s="2" t="s">
+      <c r="D74" s="2" t="s">
         <v>156</v>
       </c>
-      <c r="E73" s="2">
+      <c r="E74" s="2">
         <v>1997</v>
       </c>
-      <c r="F73" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I73" s="2" t="s">
+      <c r="F74" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I74" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="J73" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K73" s="2">
+      <c r="J74" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K74" s="2">
         <v>4</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12">
-      <c r="A76" s="2" t="s">
+      <c r="L74" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="77" spans="1:12">
+      <c r="A77" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="B76" s="2">
+      <c r="B77" s="2">
         <v>1</v>
       </c>
-      <c r="C76" s="2" t="s">
+      <c r="C77" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="D76" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="E76" s="2">
+      <c r="E77" s="2">
         <v>2014</v>
-      </c>
-      <c r="F76" s="2" t="s">
-        <v>42</v>
-      </c>
-      <c r="G76" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="H76" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I76" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="J76" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K76" s="2">
-        <v>2</v>
-      </c>
-      <c r="L76" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12">
-      <c r="B77" s="2">
-        <v>2</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="D77" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E77" s="2">
-        <v>2015</v>
       </c>
       <c r="F77" s="2" t="s">
         <v>42</v>
@@ -3821,13 +3827,13 @@
         <v>13</v>
       </c>
       <c r="I77" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J77" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K77" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L77" s="2" t="s">
         <v>31</v>
@@ -3835,54 +3841,54 @@
     </row>
     <row r="78" spans="1:12">
       <c r="B78" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="E78" s="2">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G78" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H78" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I78" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J78" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K78" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L78" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="79" spans="1:12">
       <c r="B79" s="2">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D79" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E79" s="2">
         <v>2018</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>28</v>
@@ -3894,10 +3900,10 @@
         <v>14</v>
       </c>
       <c r="J79" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K79" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L79" s="2" t="s">
         <v>15</v>
@@ -3905,83 +3911,83 @@
     </row>
     <row r="80" spans="1:12">
       <c r="B80" s="2">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D80" s="2" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="E80" s="2">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G80" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H80" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I80" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J80" s="2" t="s">
         <v>13</v>
       </c>
       <c r="K80" s="2">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L80" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="2:12">
       <c r="B81" s="2">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C81" s="2" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="D81" s="2" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="E81" s="2">
         <v>2019</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G81" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H81" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I81" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J81" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K81" s="2">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L81" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="2:12">
       <c r="B82" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C82" s="2" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="D82" s="2" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="E82" s="2">
         <v>2019</v>
@@ -3990,36 +3996,36 @@
         <v>42</v>
       </c>
       <c r="G82" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>13</v>
       </c>
       <c r="I82" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J82" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K82" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L82" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="83" spans="2:12">
       <c r="B83" s="2">
-        <v>8</v>
-      </c>
-      <c r="C83" s="5" t="s">
-        <v>162</v>
+        <v>7</v>
+      </c>
+      <c r="C83" s="2" t="s">
+        <v>160</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E83" s="2">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F83" s="2" t="s">
         <v>42</v>
@@ -4037,21 +4043,21 @@
         <v>13</v>
       </c>
       <c r="K83" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L83" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="84" spans="2:12">
       <c r="B84" s="2">
-        <v>9</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>142</v>
+        <v>8</v>
+      </c>
+      <c r="C84" s="5" t="s">
+        <v>162</v>
       </c>
       <c r="D84" s="2" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E84" s="2">
         <v>2020</v>
@@ -4066,33 +4072,33 @@
         <v>13</v>
       </c>
       <c r="I84" s="2" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J84" s="2" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K84" s="2">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L84" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="85" spans="2:12">
       <c r="B85" s="2">
-        <v>10</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>182</v>
+        <v>9</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>142</v>
       </c>
       <c r="D85" s="2" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="E85" s="2">
         <v>2020</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>13</v>
@@ -4101,15 +4107,50 @@
         <v>13</v>
       </c>
       <c r="I85" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="K85" s="2">
+        <v>5</v>
+      </c>
+      <c r="L85" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="86" spans="2:12">
+      <c r="B86" s="2">
+        <v>10</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="E86" s="2">
+        <v>2020</v>
+      </c>
+      <c r="F86" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="J85" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K85" s="2">
+      <c r="J86" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K86" s="2">
         <v>2</v>
       </c>
-      <c r="L85" s="2" t="s">
+      <c r="L86" s="2" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Bees Algorithm (Standard and Probilistic version) to swarm-based
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -1477,8 +1477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -1895,16 +1895,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>40</v>
+        <v>184</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>41</v>
+        <v>185</v>
       </c>
       <c r="E13" s="2">
-        <v>2007</v>
+        <v>2006</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>13</v>
@@ -1919,10 +1919,10 @@
         <v>13</v>
       </c>
       <c r="K13" s="2">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="14" spans="1:13">
@@ -1930,16 +1930,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>184</v>
+        <v>40</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>185</v>
+        <v>41</v>
       </c>
       <c r="E14" s="2">
-        <v>2008</v>
+        <v>2007</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>13</v>
@@ -1954,15 +1954,15 @@
         <v>13</v>
       </c>
       <c r="K14" s="2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="15" spans="1:13">
       <c r="B15" s="2">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>43</v>
@@ -1997,7 +1997,7 @@
     </row>
     <row r="16" spans="1:13">
       <c r="B16" s="2">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>45</v>
@@ -2032,7 +2032,7 @@
     </row>
     <row r="17" spans="2:12">
       <c r="B17" s="2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>176</v>
@@ -2067,7 +2067,7 @@
     </row>
     <row r="18" spans="2:12">
       <c r="B18" s="2">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>47</v>
@@ -2102,7 +2102,7 @@
     </row>
     <row r="19" spans="2:12">
       <c r="B19" s="2">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>52</v>
@@ -2137,7 +2137,7 @@
     </row>
     <row r="20" spans="2:12">
       <c r="B20" s="2">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>54</v>
@@ -2172,7 +2172,7 @@
     </row>
     <row r="21" spans="2:12">
       <c r="B21" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="C21" s="2" t="s">
         <v>56</v>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="22" spans="2:12">
       <c r="B22" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>58</v>
@@ -2242,7 +2242,7 @@
     </row>
     <row r="23" spans="2:12">
       <c r="B23" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C23" s="2" t="s">
         <v>171</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="24" spans="2:12">
       <c r="B24" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C24" s="4" t="s">
         <v>179</v>
@@ -2312,7 +2312,7 @@
     </row>
     <row r="25" spans="2:12">
       <c r="B25" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>61</v>
@@ -2347,7 +2347,7 @@
     </row>
     <row r="26" spans="2:12">
       <c r="B26" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>64</v>
@@ -2382,7 +2382,7 @@
     </row>
     <row r="27" spans="2:12">
       <c r="B27" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>172</v>
@@ -2417,7 +2417,7 @@
     </row>
     <row r="28" spans="2:12">
       <c r="B28" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>66</v>
@@ -2452,7 +2452,7 @@
     </row>
     <row r="29" spans="2:12">
       <c r="B29" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>68</v>
@@ -2487,7 +2487,7 @@
     </row>
     <row r="30" spans="2:12">
       <c r="B30" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>72</v>
@@ -2522,7 +2522,7 @@
     </row>
     <row r="31" spans="2:12">
       <c r="B31" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>78</v>
@@ -2557,7 +2557,7 @@
     </row>
     <row r="32" spans="2:12">
       <c r="B32" s="2">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>80</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="33" spans="1:12">
       <c r="B33" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>82</v>
@@ -2627,7 +2627,7 @@
     </row>
     <row r="34" spans="1:12">
       <c r="B34" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>84</v>
@@ -2662,7 +2662,7 @@
     </row>
     <row r="35" spans="1:12">
       <c r="B35" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C35" s="2" t="s">
         <v>86</v>
@@ -2697,7 +2697,7 @@
     </row>
     <row r="36" spans="1:12">
       <c r="B36" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>90</v>
@@ -2732,7 +2732,7 @@
     </row>
     <row r="37" spans="1:12">
       <c r="B37" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="C37" s="2" t="s">
         <v>92</v>

</xml_diff>

<commit_message>
Update a breakthrough version 1.1.0
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -522,9 +522,6 @@
     <t>Evolutionary</t>
   </si>
   <si>
-    <t>Fake Algorithms</t>
-  </si>
-  <si>
     <t>Probabilistic</t>
   </si>
   <si>
@@ -634,6 +631,9 @@
   </si>
   <si>
     <t>ACO-R</t>
+  </si>
+  <si>
+    <t>Dummy Algorithms</t>
   </si>
 </sst>
 </file>
@@ -1526,8 +1526,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M94"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="A87" sqref="A1:L94"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="M84" sqref="M84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1579,7 +1579,7 @@
         <v>9</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="M1" s="3"/>
     </row>
@@ -1914,10 +1914,10 @@
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="D12" s="1" t="s">
         <v>202</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>203</v>
       </c>
       <c r="E12" s="1">
         <v>2005</v>
@@ -1984,10 +1984,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>184</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>185</v>
       </c>
       <c r="E14" s="1">
         <v>2006</v>
@@ -2054,10 +2054,10 @@
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="E16" s="1">
         <v>2008</v>
@@ -2089,10 +2089,10 @@
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="D17" s="1" t="s">
         <v>200</v>
-      </c>
-      <c r="D17" s="1" t="s">
-        <v>201</v>
       </c>
       <c r="E17" s="1">
         <v>2009</v>
@@ -2194,10 +2194,10 @@
         <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="D20" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="D20" s="1" t="s">
-        <v>177</v>
       </c>
       <c r="E20" s="1">
         <v>2012</v>
@@ -2212,7 +2212,7 @@
         <v>13</v>
       </c>
       <c r="I20" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="J20" s="1" t="s">
         <v>13</v>
@@ -2404,7 +2404,7 @@
         <v>17</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D26" s="1" t="s">
         <v>60</v>
@@ -2439,16 +2439,16 @@
         <v>18</v>
       </c>
       <c r="C27" s="4" t="s">
+        <v>178</v>
+      </c>
+      <c r="D27" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="E27" s="1">
         <v>2016</v>
       </c>
       <c r="F27" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G27" s="1" t="s">
         <v>13</v>
@@ -2509,10 +2509,10 @@
         <v>20</v>
       </c>
       <c r="C29" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="D29" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="D29" s="1" t="s">
-        <v>199</v>
       </c>
       <c r="E29" s="1">
         <v>2016</v>
@@ -2579,10 +2579,10 @@
         <v>22</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D31" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="D31" s="1" t="s">
-        <v>173</v>
       </c>
       <c r="E31" s="1">
         <v>2017</v>
@@ -2614,10 +2614,10 @@
         <v>23</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>197</v>
       </c>
       <c r="E32" s="1">
         <v>2017</v>
@@ -3001,16 +3001,16 @@
     </row>
     <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44" s="1" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B44" s="1">
         <v>1</v>
       </c>
       <c r="C44" s="4" t="s">
+        <v>193</v>
+      </c>
+      <c r="D44" s="1" t="s">
         <v>194</v>
-      </c>
-      <c r="D44" s="1" t="s">
-        <v>195</v>
       </c>
       <c r="E44" s="1">
         <v>1987</v>
@@ -3330,10 +3330,10 @@
         <v>1</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="E54" s="1">
         <v>1994</v>
@@ -3365,10 +3365,10 @@
         <v>2</v>
       </c>
       <c r="C55" s="4" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>188</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>189</v>
       </c>
       <c r="E55" s="1">
         <v>2007</v>
@@ -3680,10 +3680,10 @@
         <v>11</v>
       </c>
       <c r="C64" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>175</v>
       </c>
       <c r="E64" s="1">
         <v>2020</v>
@@ -3714,60 +3714,60 @@
       <c r="B65" s="1">
         <v>12</v>
       </c>
+      <c r="C65" s="4" t="s">
+        <v>181</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="E65" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I65" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J65" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K65" s="1">
+        <v>2</v>
+      </c>
+      <c r="L65" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A66" s="1" t="s">
+      <c r="B66" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A67" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="B66" s="1">
+      <c r="B67" s="1">
         <v>1</v>
       </c>
-      <c r="C66" s="1" t="s">
+      <c r="C67" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="D66" s="1" t="s">
+      <c r="D67" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="E66" s="1">
+      <c r="E67" s="1">
         <v>2006</v>
       </c>
-      <c r="F66" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H66" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I66" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J66" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K66" s="1">
-        <v>5</v>
-      </c>
-      <c r="L66" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B67" s="1">
-        <v>2</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="E67" s="1">
-        <v>2008</v>
-      </c>
       <c r="F67" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>13</v>
@@ -3782,7 +3782,7 @@
         <v>28</v>
       </c>
       <c r="K67" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>15</v>
@@ -3790,51 +3790,51 @@
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B68" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E68" s="1">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="F68" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H68" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K68" s="1">
         <v>4</v>
       </c>
       <c r="L68" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B69" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E69" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F69" s="1" t="s">
         <v>42</v>
@@ -3846,36 +3846,36 @@
         <v>13</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K69" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L69" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B70" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>70</v>
+        <v>138</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>71</v>
+        <v>139</v>
       </c>
       <c r="E70" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F70" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H70" s="1" t="s">
         <v>13</v>
@@ -3887,24 +3887,24 @@
         <v>28</v>
       </c>
       <c r="K70" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L70" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B71" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>140</v>
+        <v>70</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>141</v>
+        <v>71</v>
       </c>
       <c r="E71" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F71" s="1" t="s">
         <v>42</v>
@@ -3922,7 +3922,7 @@
         <v>28</v>
       </c>
       <c r="K71" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>31</v>
@@ -3930,22 +3930,22 @@
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B72" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>159</v>
+        <v>141</v>
       </c>
       <c r="E72" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>13</v>
@@ -3957,73 +3957,73 @@
         <v>28</v>
       </c>
       <c r="K72" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B73" s="1">
+        <v>7</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="E73" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F73" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H73" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I73" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J73" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K73" s="1">
+        <v>3</v>
+      </c>
+      <c r="L73" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B74" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A74" s="1" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A75" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="B74" s="1">
+      <c r="B75" s="1">
         <v>1</v>
       </c>
-      <c r="C74" s="1" t="s">
+      <c r="C75" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="D74" s="1" t="s">
+      <c r="D75" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="E74" s="1">
+      <c r="E75" s="1">
         <v>2018</v>
       </c>
-      <c r="F74" s="1" t="s">
+      <c r="F75" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H74" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I74" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J74" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K74" s="1">
-        <v>4</v>
-      </c>
-      <c r="L74" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B75" s="1">
-        <v>2</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>186</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="E75" s="1">
-        <v>2012</v>
-      </c>
-      <c r="F75" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G75" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>13</v>
@@ -4035,7 +4035,7 @@
         <v>28</v>
       </c>
       <c r="K75" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>31</v>
@@ -4043,112 +4043,112 @@
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B76" s="1">
-        <v>3</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>147</v>
+        <v>2</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>148</v>
+        <v>186</v>
       </c>
       <c r="E76" s="1">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I76" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J76" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K76" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B77" s="1">
+        <v>3</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K77" s="1">
+        <v>2</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B78" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A79" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B79" s="1">
         <v>1</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C79" s="4" t="s">
+        <v>191</v>
+      </c>
+      <c r="D79" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="D78" s="1" t="s">
-        <v>193</v>
-      </c>
-      <c r="E78" s="1">
+      <c r="E79" s="1">
         <v>1993</v>
       </c>
-      <c r="F78" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I78" s="1" t="s">
+      <c r="F79" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I79" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K78" s="1">
+      <c r="J79" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K79" s="1">
         <v>3</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B79" s="1">
-        <v>2</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E79" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G79" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K79" s="1">
-        <v>2</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>15</v>
@@ -4156,145 +4156,145 @@
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B80" s="1">
+        <v>2</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E80" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F80" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G80" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I80" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J80" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K80" s="1">
+        <v>2</v>
+      </c>
+      <c r="L80" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B81" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A81" s="1" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A82" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B81" s="1">
+      <c r="B82" s="1">
         <v>1</v>
       </c>
-      <c r="C81" s="1" t="s">
+      <c r="C82" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="D81" s="1" t="s">
+      <c r="D82" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="E81" s="1">
+      <c r="E82" s="1">
         <v>2001</v>
       </c>
-      <c r="F81" s="1" t="s">
+      <c r="F82" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G81" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H81" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I81" s="1" t="s">
+      <c r="G82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J81" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K81" s="1">
+      <c r="J82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K82" s="1">
         <v>5</v>
       </c>
-      <c r="L81" s="1" t="s">
+      <c r="L82" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B82" s="1">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B83" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A83" s="1" t="s">
-        <v>168</v>
-      </c>
-      <c r="B83" s="1">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A84" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="B84" s="1">
         <v>1</v>
       </c>
-      <c r="C83" s="2" t="s">
+      <c r="C84" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E84" s="1">
         <v>1997</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="1" t="s">
+      <c r="F84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K83" s="1">
+      <c r="J84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K84" s="1">
         <v>4</v>
       </c>
-      <c r="L83" s="1" t="s">
+      <c r="L84" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B84" s="1">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B85" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B85" s="1">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A86" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B86" s="1">
         <v>1</v>
       </c>
-      <c r="C85" s="1" t="s">
+      <c r="C86" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D86" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E85" s="1">
+      <c r="E86" s="1">
         <v>2014</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K85" s="1">
-        <v>2</v>
-      </c>
-      <c r="L85" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B86" s="1">
-        <v>2</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D86" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E86" s="1">
-        <v>2015</v>
       </c>
       <c r="F86" s="1" t="s">
         <v>42</v>
@@ -4306,13 +4306,13 @@
         <v>13</v>
       </c>
       <c r="I86" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J86" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K86" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L86" s="1" t="s">
         <v>31</v>
@@ -4320,54 +4320,54 @@
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B87" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>74</v>
+        <v>134</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>75</v>
+        <v>135</v>
       </c>
       <c r="E87" s="1">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H87" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I87" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J87" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K87" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L87" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B88" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E88" s="1">
         <v>2018</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G88" s="1" t="s">
         <v>28</v>
@@ -4379,10 +4379,10 @@
         <v>14</v>
       </c>
       <c r="J88" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K88" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L88" s="1" t="s">
         <v>15</v>
@@ -4390,83 +4390,83 @@
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B89" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>165</v>
+        <v>76</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>164</v>
+        <v>77</v>
       </c>
       <c r="E89" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H89" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K89" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L89" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B90" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>88</v>
+        <v>165</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>89</v>
+        <v>164</v>
       </c>
       <c r="E90" s="1">
         <v>2019</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H90" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J90" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K90" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L90" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="91" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B91" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>160</v>
+        <v>88</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>161</v>
+        <v>89</v>
       </c>
       <c r="E91" s="1">
         <v>2019</v>
@@ -4475,36 +4475,36 @@
         <v>42</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H91" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J91" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K91" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L91" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="92" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B92" s="1">
-        <v>8</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>162</v>
+        <v>7</v>
+      </c>
+      <c r="C92" s="1" t="s">
+        <v>160</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="E92" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>42</v>
@@ -4522,21 +4522,21 @@
         <v>13</v>
       </c>
       <c r="K92" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B93" s="1">
-        <v>9</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>142</v>
+        <v>8</v>
+      </c>
+      <c r="C93" s="2" t="s">
+        <v>162</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="E93" s="1">
         <v>2020</v>
@@ -4551,33 +4551,33 @@
         <v>13</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K93" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="94" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B94" s="1">
-        <v>10</v>
-      </c>
-      <c r="C94" s="4" t="s">
-        <v>182</v>
+        <v>9</v>
+      </c>
+      <c r="C94" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>183</v>
+        <v>143</v>
       </c>
       <c r="E94" s="1">
         <v>2020</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>13</v>
@@ -4586,13 +4586,13 @@
         <v>13</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K94" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>31</v>

</xml_diff>

<commit_message>
Add Arithmetic Optimization Algorithm (AOA) to Math-based group
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="209">
   <si>
     <t>Group</t>
   </si>
@@ -303,9 +303,6 @@
     <t>SpaSA</t>
   </si>
   <si>
-    <t>BEST</t>
-  </si>
-  <si>
     <t>Wind Driven Optimization</t>
   </si>
   <si>
@@ -552,9 +549,6 @@
     <t>FOA</t>
   </si>
   <si>
-    <t>WEAK</t>
-  </si>
-  <si>
     <t>Jaya Algorithm</t>
   </si>
   <si>
@@ -646,13 +640,19 @@
   </si>
   <si>
     <t>CSA</t>
+  </si>
+  <si>
+    <t>Arithmetic Optimization Algorithm</t>
+  </si>
+  <si>
+    <t>AOA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="23" x14ac:knownFonts="1">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -821,6 +821,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF080808"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="33">
@@ -1164,7 +1171,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1179,6 +1186,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1536,13 +1546,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M96"/>
+  <dimension ref="A1:M97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="O78" sqref="O78"/>
+    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
+      <selection activeCell="N85" sqref="N85"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15.6"/>
   <cols>
     <col min="1" max="1" width="20.5546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="8.88671875" style="1"/>
@@ -1556,7 +1566,7 @@
     <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" ht="18">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -1585,19 +1595,19 @@
         <v>8</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="K1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13">
       <c r="A2" s="1" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -1633,7 +1643,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13">
       <c r="B3" s="1">
         <v>2</v>
       </c>
@@ -1668,7 +1678,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13">
       <c r="B4" s="1">
         <v>3</v>
       </c>
@@ -1703,7 +1713,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13">
       <c r="B5" s="1">
         <v>3</v>
       </c>
@@ -1738,7 +1748,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13">
       <c r="B6" s="1">
         <v>4</v>
       </c>
@@ -1773,7 +1783,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13">
       <c r="B7" s="1">
         <v>5</v>
       </c>
@@ -1808,7 +1818,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13">
       <c r="B8" s="1">
         <v>6</v>
       </c>
@@ -1843,12 +1853,12 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13">
       <c r="B9" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13">
       <c r="A10" s="1" t="s">
         <v>32</v>
       </c>
@@ -1886,7 +1896,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13">
       <c r="B11" s="1">
         <v>2</v>
       </c>
@@ -1921,15 +1931,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13">
       <c r="B12" s="1">
         <v>3</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="E12" s="1">
         <v>2005</v>
@@ -1956,7 +1966,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13">
       <c r="B13" s="1">
         <v>4</v>
       </c>
@@ -1991,15 +2001,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13">
       <c r="B14" s="1">
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D14" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E14" s="1">
         <v>2006</v>
@@ -2026,7 +2036,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13">
       <c r="B15" s="1">
         <v>6</v>
       </c>
@@ -2061,15 +2071,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13">
       <c r="B16" s="1">
         <v>7</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="E16" s="1">
         <v>2008</v>
@@ -2096,15 +2106,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:12">
       <c r="B17" s="1">
         <v>8</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D17" s="1" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E17" s="1">
         <v>2009</v>
@@ -2131,15 +2141,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12">
       <c r="B18" s="1">
         <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E18" s="1">
         <v>2009</v>
@@ -2166,7 +2176,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="19" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12">
       <c r="B19" s="1">
         <v>10</v>
       </c>
@@ -2201,7 +2211,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="20" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12">
       <c r="B20" s="1">
         <v>11</v>
       </c>
@@ -2236,15 +2246,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="21" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:12">
       <c r="B21" s="1">
         <v>12</v>
       </c>
       <c r="C21" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D21" s="1" t="s">
         <v>175</v>
-      </c>
-      <c r="D21" s="1" t="s">
-        <v>176</v>
       </c>
       <c r="E21" s="1">
         <v>2012</v>
@@ -2259,7 +2269,7 @@
         <v>13</v>
       </c>
       <c r="I21" s="1" t="s">
-        <v>177</v>
+        <v>20</v>
       </c>
       <c r="J21" s="1" t="s">
         <v>13</v>
@@ -2271,7 +2281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="22" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:12">
       <c r="B22" s="1">
         <v>13</v>
       </c>
@@ -2306,7 +2316,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12">
       <c r="B23" s="1">
         <v>14</v>
       </c>
@@ -2341,7 +2351,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12">
       <c r="B24" s="1">
         <v>15</v>
       </c>
@@ -2376,7 +2386,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12">
       <c r="B25" s="1">
         <v>16</v>
       </c>
@@ -2411,7 +2421,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:12">
       <c r="B26" s="1">
         <v>17</v>
       </c>
@@ -2446,12 +2456,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="27" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:12">
       <c r="B27" s="1">
         <v>18</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D27" s="1" t="s">
         <v>60</v>
@@ -2481,21 +2491,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="28" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:12">
       <c r="B28" s="1">
         <v>19</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D28" s="1" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E28" s="1">
         <v>2016</v>
       </c>
       <c r="F28" s="1" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="G28" s="1" t="s">
         <v>13</v>
@@ -2516,7 +2526,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="29" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:12">
       <c r="B29" s="1">
         <v>20</v>
       </c>
@@ -2539,7 +2549,7 @@
         <v>13</v>
       </c>
       <c r="I29" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J29" s="1" t="s">
         <v>28</v>
@@ -2551,15 +2561,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="30" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:12">
       <c r="B30" s="1">
         <v>21</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D30" s="1" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="E30" s="1">
         <v>2016</v>
@@ -2586,7 +2596,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="31" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:12">
       <c r="B31" s="1">
         <v>22</v>
       </c>
@@ -2621,15 +2631,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="32" spans="2:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:12">
       <c r="B32" s="1">
         <v>23</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="D32" s="1" t="s">
-        <v>172</v>
       </c>
       <c r="E32" s="1">
         <v>2017</v>
@@ -2656,15 +2666,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12">
       <c r="B33" s="1">
         <v>24</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="E33" s="1">
         <v>2017</v>
@@ -2691,7 +2701,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12">
       <c r="B34" s="1">
         <v>25</v>
       </c>
@@ -2726,7 +2736,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12">
       <c r="B35" s="1">
         <v>26</v>
       </c>
@@ -2761,7 +2771,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12">
       <c r="B36" s="1">
         <v>27</v>
       </c>
@@ -2796,7 +2806,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12">
       <c r="B37" s="1">
         <v>28</v>
       </c>
@@ -2831,7 +2841,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:12">
       <c r="B38" s="1">
         <v>29</v>
       </c>
@@ -2866,7 +2876,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:12">
       <c r="B39" s="1">
         <v>30</v>
       </c>
@@ -2901,7 +2911,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:12">
       <c r="B40" s="1">
         <v>31</v>
       </c>
@@ -2936,7 +2946,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:12">
       <c r="B41" s="1">
         <v>32</v>
       </c>
@@ -2959,7 +2969,7 @@
         <v>13</v>
       </c>
       <c r="I41" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J41" s="1" t="s">
         <v>28</v>
@@ -2971,7 +2981,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12">
       <c r="B42" s="1">
         <v>33</v>
       </c>
@@ -3006,7 +3016,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:12">
       <c r="B43" s="1">
         <v>34</v>
       </c>
@@ -3041,7 +3051,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:12">
       <c r="B44" s="1">
         <v>35</v>
       </c>
@@ -3064,7 +3074,7 @@
         <v>13</v>
       </c>
       <c r="I44" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J44" s="1" t="s">
         <v>28</v>
@@ -3076,15 +3086,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:12">
       <c r="B45" s="1">
         <v>36</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="E45" s="1">
         <v>2021</v>
@@ -3099,7 +3109,7 @@
         <v>13</v>
       </c>
       <c r="I45" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J45" s="1" t="s">
         <v>28</v>
@@ -3111,23 +3121,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:12">
       <c r="B46" s="1">
         <v>37</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:12">
       <c r="A47" s="1" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="D47" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="E47" s="1">
         <v>1987</v>
@@ -3154,15 +3164,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:12">
       <c r="B48" s="1">
         <v>2</v>
       </c>
       <c r="C48" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D48" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="E48" s="1">
         <v>2013</v>
@@ -3189,15 +3199,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:12">
       <c r="B49" s="1">
         <v>3</v>
       </c>
       <c r="C49" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D49" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="E49" s="1">
         <v>2016</v>
@@ -3224,21 +3234,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:12">
       <c r="B50" s="1">
         <v>4</v>
       </c>
       <c r="C50" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D50" s="1" t="s">
         <v>99</v>
-      </c>
-      <c r="D50" s="1" t="s">
-        <v>100</v>
       </c>
       <c r="E50" s="1">
         <v>2016</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G50" s="1" t="s">
         <v>13</v>
@@ -3259,15 +3269,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:12">
       <c r="B51" s="1">
         <v>5</v>
       </c>
       <c r="C51" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D51" s="1" t="s">
         <v>102</v>
-      </c>
-      <c r="D51" s="1" t="s">
-        <v>103</v>
       </c>
       <c r="E51" s="1">
         <v>2016</v>
@@ -3294,21 +3304,21 @@
         <v>15</v>
       </c>
     </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:12">
       <c r="B52" s="1">
         <v>6</v>
       </c>
       <c r="C52" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" s="1" t="s">
         <v>104</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>105</v>
       </c>
       <c r="E52" s="1">
         <v>2019</v>
       </c>
       <c r="F52" s="1" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G52" s="1" t="s">
         <v>13</v>
@@ -3329,15 +3339,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:12">
       <c r="B53" s="1">
         <v>7</v>
       </c>
       <c r="C53" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="D53" s="1" t="s">
         <v>106</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>107</v>
       </c>
       <c r="E53" s="1">
         <v>2019</v>
@@ -3364,15 +3374,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:12">
       <c r="B54" s="1">
         <v>8</v>
       </c>
       <c r="C54" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="D54" s="1" t="s">
         <v>108</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>109</v>
       </c>
       <c r="E54" s="1">
         <v>2019</v>
@@ -3399,15 +3409,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:12">
       <c r="B55" s="1">
         <v>9</v>
       </c>
       <c r="C55" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="E55" s="1">
         <v>2019</v>
@@ -3422,7 +3432,7 @@
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J55" s="1" t="s">
         <v>28</v>
@@ -3434,23 +3444,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:12">
       <c r="B56" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:12">
       <c r="A57" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B57" s="1">
         <v>1</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="E57" s="1">
         <v>1994</v>
@@ -3477,15 +3487,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:12">
       <c r="B58" s="1">
         <v>2</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="E58" s="1">
         <v>2007</v>
@@ -3512,15 +3522,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:12">
       <c r="B59" s="1">
         <v>3</v>
       </c>
       <c r="C59" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D59" s="1" t="s">
         <v>113</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>114</v>
       </c>
       <c r="E59" s="1">
         <v>2011</v>
@@ -3547,15 +3557,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:12">
       <c r="B60" s="1">
         <v>4</v>
       </c>
       <c r="C60" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D60" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="D60" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="E60" s="1">
         <v>2011</v>
@@ -3582,15 +3592,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:12">
       <c r="B61" s="1">
         <v>5</v>
       </c>
       <c r="C61" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D61" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D61" s="1" t="s">
-        <v>118</v>
       </c>
       <c r="E61" s="1">
         <v>2019</v>
@@ -3617,15 +3627,15 @@
         <v>37</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:12">
       <c r="B62" s="1">
         <v>6</v>
       </c>
       <c r="C62" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="D62" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="E62" s="1">
         <v>2019</v>
@@ -3652,15 +3662,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:12">
       <c r="B63" s="1">
         <v>7</v>
       </c>
       <c r="C63" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D63" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="D63" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="E63" s="1">
         <v>2019</v>
@@ -3687,15 +3697,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:12">
       <c r="B64" s="1">
         <v>8</v>
       </c>
       <c r="C64" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="D64" s="1" t="s">
         <v>123</v>
-      </c>
-      <c r="D64" s="1" t="s">
-        <v>124</v>
       </c>
       <c r="E64" s="1">
         <v>2019</v>
@@ -3710,7 +3720,7 @@
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>94</v>
+        <v>63</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>28</v>
@@ -3722,15 +3732,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:12">
       <c r="B65" s="1">
         <v>9</v>
       </c>
       <c r="C65" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="D65" s="1" t="s">
         <v>125</v>
-      </c>
-      <c r="D65" s="1" t="s">
-        <v>126</v>
       </c>
       <c r="E65" s="1">
         <v>2019</v>
@@ -3757,15 +3767,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:12">
       <c r="B66" s="1">
         <v>10</v>
       </c>
       <c r="C66" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D66" s="1" t="s">
         <v>127</v>
-      </c>
-      <c r="D66" s="1" t="s">
-        <v>128</v>
       </c>
       <c r="E66" s="1">
         <v>2020</v>
@@ -3792,15 +3802,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:12">
       <c r="B67" s="1">
         <v>11</v>
       </c>
       <c r="C67" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D67" s="1" t="s">
         <v>173</v>
-      </c>
-      <c r="D67" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="E67" s="1">
         <v>2020</v>
@@ -3827,15 +3837,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:12">
       <c r="B68" s="1">
         <v>12</v>
       </c>
       <c r="C68" s="4" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="E68" s="1">
         <v>2020</v>
@@ -3862,23 +3872,23 @@
         <v>31</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:12">
       <c r="B69" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:12">
       <c r="A70" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B70" s="1">
         <v>1</v>
       </c>
       <c r="C70" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="D70" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="D70" s="1" t="s">
-        <v>131</v>
       </c>
       <c r="E70" s="1">
         <v>2006</v>
@@ -3905,15 +3915,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:12">
       <c r="B71" s="1">
         <v>2</v>
       </c>
       <c r="C71" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D71" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>133</v>
       </c>
       <c r="E71" s="1">
         <v>2008</v>
@@ -3940,15 +3950,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:12">
       <c r="B72" s="1">
         <v>3</v>
       </c>
       <c r="C72" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="D72" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>137</v>
       </c>
       <c r="E72" s="1">
         <v>2016</v>
@@ -3975,15 +3985,15 @@
         <v>49</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:12">
       <c r="B73" s="1">
         <v>4</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D73" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="D73" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="E73" s="1">
         <v>2017</v>
@@ -4010,7 +4020,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:12">
       <c r="B74" s="1">
         <v>5</v>
       </c>
@@ -4045,15 +4055,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:12">
       <c r="B75" s="1">
         <v>6</v>
       </c>
       <c r="C75" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="D75" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="D75" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="E75" s="1">
         <v>2019</v>
@@ -4080,15 +4090,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:12">
       <c r="B76" s="1">
         <v>7</v>
       </c>
       <c r="C76" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D76" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D76" s="1" t="s">
-        <v>159</v>
       </c>
       <c r="E76" s="1">
         <v>2020</v>
@@ -4115,23 +4125,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:12">
       <c r="B77" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:12">
       <c r="A78" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B78" s="1">
         <v>1</v>
       </c>
       <c r="C78" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="D78" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="D78" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E78" s="1">
         <v>2018</v>
@@ -4158,15 +4168,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:12">
       <c r="B79" s="1">
         <v>2</v>
       </c>
       <c r="C79" s="4" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E79" s="1">
         <v>2012</v>
@@ -4193,15 +4203,15 @@
         <v>31</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:12">
       <c r="B80" s="1">
         <v>3</v>
       </c>
       <c r="C80" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D80" s="1" t="s">
         <v>147</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="E80" s="1">
         <v>2019</v>
@@ -4228,23 +4238,23 @@
         <v>15</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:12">
       <c r="B81" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:12">
       <c r="A82" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B82" s="1">
         <v>1</v>
       </c>
       <c r="C82" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="E82" s="1">
         <v>1993</v>
@@ -4271,15 +4281,15 @@
         <v>15</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:12">
       <c r="B83" s="1">
         <v>2</v>
       </c>
       <c r="C83" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D83" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="E83" s="1">
         <v>2016</v>
@@ -4306,147 +4316,147 @@
         <v>15</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:12">
       <c r="B84" s="1">
         <v>3</v>
       </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A85" s="1" t="s">
+      <c r="C84" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E84" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J84" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K84" s="1">
+        <v>6</v>
+      </c>
+      <c r="L84" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="85" spans="1:12">
+      <c r="B85" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="A86" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B86" s="1">
+        <v>1</v>
+      </c>
+      <c r="C86" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="B85" s="1">
+      <c r="D86" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2001</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K86" s="1">
+        <v>5</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="B87" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="88" spans="1:12">
+      <c r="A88" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B88" s="1">
         <v>1</v>
       </c>
-      <c r="C85" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="D85" s="1" t="s">
+      <c r="C88" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E85" s="1">
-        <v>2001</v>
-      </c>
-      <c r="F85" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G85" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I85" s="1" t="s">
+      <c r="D88" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E88" s="1">
+        <v>1997</v>
+      </c>
+      <c r="F88" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J85" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K85" s="1">
-        <v>5</v>
-      </c>
-      <c r="L85" s="1" t="s">
+      <c r="J88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K88" s="1">
+        <v>4</v>
+      </c>
+      <c r="L88" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B86" s="1">
+    <row r="89" spans="1:12">
+      <c r="B89" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A87" s="1" t="s">
-        <v>167</v>
-      </c>
-      <c r="B87" s="1">
+    <row r="90" spans="1:12">
+      <c r="A90" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B90" s="1">
         <v>1</v>
       </c>
-      <c r="C87" s="2" t="s">
-        <v>155</v>
-      </c>
-      <c r="D87" s="1" t="s">
-        <v>156</v>
-      </c>
-      <c r="E87" s="1">
-        <v>1997</v>
-      </c>
-      <c r="F87" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K87" s="1">
-        <v>4</v>
-      </c>
-      <c r="L87" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B88" s="1">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A89" s="1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B89" s="1">
-        <v>1</v>
-      </c>
-      <c r="C89" s="1" t="s">
+      <c r="C90" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E90" s="1">
         <v>2014</v>
-      </c>
-      <c r="F89" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I89" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K89" s="1">
-        <v>2</v>
-      </c>
-      <c r="L89" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B90" s="1">
-        <v>2</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D90" s="1" t="s">
-        <v>135</v>
-      </c>
-      <c r="E90" s="1">
-        <v>2015</v>
       </c>
       <c r="F90" s="1" t="s">
         <v>42</v>
@@ -4458,68 +4468,68 @@
         <v>13</v>
       </c>
       <c r="I90" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J90" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K90" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L90" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:12">
       <c r="B91" s="1">
+        <v>2</v>
+      </c>
+      <c r="C91" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="E91" s="1">
+        <v>2015</v>
+      </c>
+      <c r="F91" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I91" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J91" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K91" s="1">
+        <v>5</v>
+      </c>
+      <c r="L91" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="92" spans="1:12">
+      <c r="B92" s="1">
         <v>3</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="E91" s="1">
-        <v>2018</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K91" s="1">
-        <v>6</v>
-      </c>
-      <c r="L91" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B92" s="1">
-        <v>4</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>77</v>
       </c>
       <c r="E92" s="1">
         <v>2018</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G92" s="1" t="s">
         <v>28</v>
@@ -4531,65 +4541,65 @@
         <v>14</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K92" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:12">
       <c r="B93" s="1">
+        <v>4</v>
+      </c>
+      <c r="C93" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="E93" s="1">
+        <v>2018</v>
+      </c>
+      <c r="F93" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G93" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I93" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J93" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K93" s="1">
+        <v>2</v>
+      </c>
+      <c r="L93" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12">
+      <c r="B94" s="1">
         <v>5</v>
       </c>
-      <c r="C93" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="D93" s="1" t="s">
+      <c r="C94" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E93" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F93" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G93" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H93" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I93" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J93" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K93" s="1">
-        <v>6</v>
-      </c>
-      <c r="L93" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="B94" s="1">
-        <v>6</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>160</v>
-      </c>
       <c r="D94" s="1" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E94" s="1">
         <v>2019</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>13</v>
@@ -4604,24 +4614,24 @@
         <v>13</v>
       </c>
       <c r="K94" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:12">
       <c r="B95" s="1">
-        <v>7</v>
-      </c>
-      <c r="C95" s="2" t="s">
-        <v>162</v>
+        <v>6</v>
+      </c>
+      <c r="C95" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E95" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F95" s="1" t="s">
         <v>42</v>
@@ -4639,21 +4649,21 @@
         <v>13</v>
       </c>
       <c r="K95" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.3">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="96" spans="1:12">
       <c r="B96" s="1">
-        <v>8</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>142</v>
+        <v>7</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="E96" s="1">
         <v>2020</v>
@@ -4668,15 +4678,50 @@
         <v>13</v>
       </c>
       <c r="I96" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J96" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K96" s="1">
+        <v>2</v>
+      </c>
+      <c r="L96" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="97" spans="2:12">
+      <c r="B97" s="1">
+        <v>8</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E97" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F97" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I97" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J96" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K96" s="1">
+      <c r="J97" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K97" s="1">
         <v>5</v>
       </c>
-      <c r="L96" s="1" t="s">
+      <c r="L97" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Aquila Optimization (AO) to Swarm-based group
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="211">
   <si>
     <t>Group</t>
   </si>
@@ -646,6 +646,12 @@
   </si>
   <si>
     <t>AOA</t>
+  </si>
+  <si>
+    <t>Aquila Optimizer</t>
+  </si>
+  <si>
+    <t>AO</t>
   </si>
 </sst>
 </file>
@@ -1546,10 +1552,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M97"/>
+  <dimension ref="A1:M98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="N85" sqref="N85"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -3125,95 +3131,95 @@
       <c r="B46" s="1">
         <v>37</v>
       </c>
+      <c r="C46" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="E46" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F46" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J46" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K46" s="1">
+        <v>2</v>
+      </c>
+      <c r="L46" s="1" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="47" spans="1:12">
-      <c r="A47" s="1" t="s">
+      <c r="B47" s="1">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="B47" s="1">
+      <c r="B48" s="1">
         <v>1</v>
       </c>
-      <c r="C47" s="4" t="s">
+      <c r="C48" s="4" t="s">
         <v>191</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="D48" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E47" s="1">
+      <c r="E48" s="1">
         <v>1987</v>
       </c>
-      <c r="F47" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I47" s="1" t="s">
+      <c r="F48" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I48" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J47" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K47" s="1">
+      <c r="J48" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K48" s="1">
         <v>9</v>
       </c>
-      <c r="L47" s="1" t="s">
+      <c r="L48" s="1" t="s">
         <v>31</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12">
-      <c r="B48" s="1">
-        <v>2</v>
-      </c>
-      <c r="C48" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="E48" s="1">
-        <v>2013</v>
-      </c>
-      <c r="F48" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I48" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J48" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K48" s="1">
-        <v>7</v>
-      </c>
-      <c r="L48" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="49" spans="1:12">
       <c r="B49" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E49" s="1">
-        <v>2016</v>
+        <v>2013</v>
       </c>
       <c r="F49" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G49" s="1" t="s">
         <v>28</v>
@@ -3222,13 +3228,13 @@
         <v>13</v>
       </c>
       <c r="I49" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J49" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K49" s="1">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="L49" s="1" t="s">
         <v>15</v>
@@ -3236,34 +3242,34 @@
     </row>
     <row r="50" spans="1:12">
       <c r="B50" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E50" s="1">
         <v>2016</v>
       </c>
       <c r="F50" s="1" t="s">
-        <v>100</v>
+        <v>42</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I50" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J50" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K50" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L50" s="1" t="s">
         <v>15</v>
@@ -3271,22 +3277,22 @@
     </row>
     <row r="51" spans="1:12">
       <c r="B51" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E51" s="1">
         <v>2016</v>
       </c>
       <c r="F51" s="1" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H51" s="1" t="s">
         <v>13</v>
@@ -3295,10 +3301,10 @@
         <v>14</v>
       </c>
       <c r="J51" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K51" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L51" s="1" t="s">
         <v>15</v>
@@ -3306,60 +3312,60 @@
     </row>
     <row r="52" spans="1:12">
       <c r="B52" s="1">
+        <v>5</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E52" s="1">
+        <v>2016</v>
+      </c>
+      <c r="F52" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I52" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J52" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K52" s="1">
         <v>6</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="E52" s="1">
-        <v>2019</v>
-      </c>
-      <c r="F52" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="G52" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I52" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="J52" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K52" s="1">
-        <v>2</v>
-      </c>
       <c r="L52" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="53" spans="1:12">
       <c r="B53" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E53" s="1">
         <v>2019</v>
       </c>
       <c r="F53" s="1" t="s">
-        <v>12</v>
+        <v>100</v>
       </c>
       <c r="G53" s="1" t="s">
         <v>13</v>
       </c>
       <c r="H53" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="I53" s="1" t="s">
         <v>63</v>
@@ -3368,21 +3374,21 @@
         <v>28</v>
       </c>
       <c r="K53" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L53" s="1" t="s">
-        <v>31</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:12">
       <c r="B54" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E54" s="1">
         <v>2019</v>
@@ -3397,13 +3403,13 @@
         <v>13</v>
       </c>
       <c r="I54" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J54" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K54" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="L54" s="1" t="s">
         <v>31</v>
@@ -3411,13 +3417,13 @@
     </row>
     <row r="55" spans="1:12">
       <c r="B55" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E55" s="1">
         <v>2019</v>
@@ -3432,73 +3438,73 @@
         <v>13</v>
       </c>
       <c r="I55" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J55" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K55" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L55" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="56" spans="1:12">
       <c r="B56" s="1">
+        <v>9</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E56" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F56" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H56" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I56" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J56" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" s="1">
+        <v>2</v>
+      </c>
+      <c r="L56" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="57" spans="1:12">
+      <c r="B57" s="1">
         <v>10</v>
       </c>
     </row>
-    <row r="57" spans="1:12">
-      <c r="A57" s="1" t="s">
+    <row r="58" spans="1:12">
+      <c r="A58" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B57" s="1">
+      <c r="B58" s="1">
         <v>1</v>
       </c>
-      <c r="C57" s="1" t="s">
+      <c r="C58" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D57" s="1" t="s">
+      <c r="D58" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E57" s="1">
+      <c r="E58" s="1">
         <v>1994</v>
-      </c>
-      <c r="F57" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J57" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K57" s="1">
-        <v>3</v>
-      </c>
-      <c r="L57" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12">
-      <c r="B58" s="1">
-        <v>2</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D58" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E58" s="1">
-        <v>2007</v>
       </c>
       <c r="F58" s="1" t="s">
         <v>12</v>
@@ -3513,59 +3519,59 @@
         <v>14</v>
       </c>
       <c r="J58" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K58" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L58" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="59" spans="1:12">
       <c r="B59" s="1">
-        <v>3</v>
-      </c>
-      <c r="C59" s="1" t="s">
-        <v>112</v>
+        <v>2</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="E59" s="1">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H59" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I59" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J59" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K59" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E60" s="1">
         <v>2011</v>
@@ -3574,39 +3580,39 @@
         <v>12</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J60" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K60" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="B61" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E61" s="1">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G61" s="1" t="s">
         <v>13</v>
@@ -3615,36 +3621,36 @@
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K61" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="B62" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E62" s="1">
         <v>2019</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H62" s="1" t="s">
         <v>13</v>
@@ -3656,21 +3662,21 @@
         <v>28</v>
       </c>
       <c r="K62" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="B63" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E63" s="1">
         <v>2019</v>
@@ -3691,21 +3697,21 @@
         <v>28</v>
       </c>
       <c r="K63" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="B64" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E64" s="1">
         <v>2019</v>
@@ -3714,13 +3720,13 @@
         <v>12</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H64" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I64" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J64" s="1" t="s">
         <v>28</v>
@@ -3734,13 +3740,13 @@
     </row>
     <row r="65" spans="1:12">
       <c r="B65" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E65" s="1">
         <v>2019</v>
@@ -3755,13 +3761,13 @@
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J65" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K65" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L65" s="1" t="s">
         <v>15</v>
@@ -3769,19 +3775,19 @@
     </row>
     <row r="66" spans="1:12">
       <c r="B66" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E66" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G66" s="1" t="s">
         <v>13</v>
@@ -3790,33 +3796,33 @@
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J66" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K66" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L66" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:12">
       <c r="B67" s="1">
-        <v>11</v>
-      </c>
-      <c r="C67" s="3" t="s">
-        <v>172</v>
+        <v>10</v>
+      </c>
+      <c r="C67" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="E67" s="1">
         <v>2020</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>13</v>
@@ -3825,13 +3831,13 @@
         <v>13</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J67" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K67" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L67" s="1" t="s">
         <v>31</v>
@@ -3839,13 +3845,13 @@
     </row>
     <row r="68" spans="1:12">
       <c r="B68" s="1">
-        <v>12</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>179</v>
+        <v>11</v>
+      </c>
+      <c r="C68" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E68" s="1">
         <v>2020</v>
@@ -3860,10 +3866,10 @@
         <v>13</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K68" s="1">
         <v>2</v>
@@ -3874,62 +3880,62 @@
     </row>
     <row r="69" spans="1:12">
       <c r="B69" s="1">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C69" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E69" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F69" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I69" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J69" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K69" s="1">
+        <v>2</v>
+      </c>
+      <c r="L69" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="70" spans="1:12">
-      <c r="A70" s="1" t="s">
+      <c r="B70" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="1:12">
+      <c r="A71" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B70" s="1">
+      <c r="B71" s="1">
         <v>1</v>
       </c>
-      <c r="C70" s="1" t="s">
+      <c r="C71" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D70" s="1" t="s">
+      <c r="D71" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E70" s="1">
+      <c r="E71" s="1">
         <v>2006</v>
       </c>
-      <c r="F70" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K70" s="1">
-        <v>5</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12">
-      <c r="B71" s="1">
-        <v>2</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E71" s="1">
-        <v>2008</v>
-      </c>
       <c r="F71" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G71" s="1" t="s">
         <v>13</v>
@@ -3944,7 +3950,7 @@
         <v>28</v>
       </c>
       <c r="K71" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L71" s="1" t="s">
         <v>15</v>
@@ -3952,51 +3958,51 @@
     </row>
     <row r="72" spans="1:12">
       <c r="B72" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E72" s="1">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="F72" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H72" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I72" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J72" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K72" s="1">
         <v>4</v>
       </c>
       <c r="L72" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:12">
       <c r="B73" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E73" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>42</v>
@@ -4008,36 +4014,36 @@
         <v>13</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K73" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="B74" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="E74" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H74" s="1" t="s">
         <v>13</v>
@@ -4049,24 +4055,24 @@
         <v>28</v>
       </c>
       <c r="K74" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="75" spans="1:12">
       <c r="B75" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="E75" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>42</v>
@@ -4084,7 +4090,7 @@
         <v>28</v>
       </c>
       <c r="K75" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L75" s="1" t="s">
         <v>31</v>
@@ -4092,22 +4098,22 @@
     </row>
     <row r="76" spans="1:12">
       <c r="B76" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E76" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H76" s="1" t="s">
         <v>13</v>
@@ -4119,73 +4125,73 @@
         <v>28</v>
       </c>
       <c r="K76" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L76" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="77" spans="1:12">
       <c r="B77" s="1">
+        <v>7</v>
+      </c>
+      <c r="C77" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E77" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F77" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H77" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I77" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J77" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K77" s="1">
+        <v>3</v>
+      </c>
+      <c r="L77" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="78" spans="1:12">
+      <c r="B78" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="78" spans="1:12">
-      <c r="A78" s="1" t="s">
+    <row r="79" spans="1:12">
+      <c r="A79" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B78" s="1">
+      <c r="B79" s="1">
         <v>1</v>
       </c>
-      <c r="C78" s="1" t="s">
+      <c r="C79" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D78" s="1" t="s">
+      <c r="D79" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E78" s="1">
+      <c r="E79" s="1">
         <v>2018</v>
       </c>
-      <c r="F78" s="1" t="s">
+      <c r="F79" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H78" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I78" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J78" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K78" s="1">
-        <v>4</v>
-      </c>
-      <c r="L78" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12">
-      <c r="B79" s="1">
-        <v>2</v>
-      </c>
-      <c r="C79" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D79" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E79" s="1">
-        <v>2012</v>
-      </c>
-      <c r="F79" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G79" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H79" s="1" t="s">
         <v>13</v>
@@ -4197,7 +4203,7 @@
         <v>28</v>
       </c>
       <c r="K79" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L79" s="1" t="s">
         <v>31</v>
@@ -4205,112 +4211,112 @@
     </row>
     <row r="80" spans="1:12">
       <c r="B80" s="1">
-        <v>3</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>146</v>
+        <v>2</v>
+      </c>
+      <c r="C80" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="E80" s="1">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I80" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J80" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K80" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L80" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="81" spans="1:12">
       <c r="B81" s="1">
+        <v>3</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E81" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F81" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G81" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H81" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I81" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J81" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K81" s="1">
+        <v>2</v>
+      </c>
+      <c r="L81" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="82" spans="1:12">
+      <c r="B82" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:12">
-      <c r="A82" s="1" t="s">
+    <row r="83" spans="1:12">
+      <c r="A83" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B82" s="1">
+      <c r="B83" s="1">
         <v>1</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C83" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D82" s="1" t="s">
+      <c r="D83" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E82" s="1">
+      <c r="E83" s="1">
         <v>1993</v>
       </c>
-      <c r="F82" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G82" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H82" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I82" s="1" t="s">
+      <c r="F83" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I83" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J82" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K82" s="1">
+      <c r="J83" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K83" s="1">
         <v>3</v>
-      </c>
-      <c r="L82" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="83" spans="1:12">
-      <c r="B83" s="1">
-        <v>2</v>
-      </c>
-      <c r="C83" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D83" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E83" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F83" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K83" s="1">
-        <v>2</v>
       </c>
       <c r="L83" s="1" t="s">
         <v>15</v>
@@ -4318,22 +4324,22 @@
     </row>
     <row r="84" spans="1:12">
       <c r="B84" s="1">
-        <v>3</v>
-      </c>
-      <c r="C84" s="6" t="s">
-        <v>207</v>
+        <v>2</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="E84" s="1">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H84" s="1" t="s">
         <v>13</v>
@@ -4342,10 +4348,10 @@
         <v>14</v>
       </c>
       <c r="J84" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K84" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>15</v>
@@ -4353,145 +4359,145 @@
     </row>
     <row r="85" spans="1:12">
       <c r="B85" s="1">
+        <v>3</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E85" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F85" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H85" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I85" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J85" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K85" s="1">
+        <v>6</v>
+      </c>
+      <c r="L85" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="86" spans="1:12">
+      <c r="B86" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="86" spans="1:12">
-      <c r="A86" s="1" t="s">
+    <row r="87" spans="1:12">
+      <c r="A87" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B86" s="1">
+      <c r="B87" s="1">
         <v>1</v>
       </c>
-      <c r="C86" s="1" t="s">
+      <c r="C87" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D86" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E86" s="1">
+      <c r="E87" s="1">
         <v>2001</v>
       </c>
-      <c r="F86" s="1" t="s">
+      <c r="F87" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G86" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H86" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I86" s="1" t="s">
+      <c r="G87" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I87" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J86" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K86" s="1">
+      <c r="J87" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K87" s="1">
         <v>5</v>
       </c>
-      <c r="L86" s="1" t="s">
+      <c r="L87" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
-      <c r="B87" s="1">
+    <row r="88" spans="1:12">
+      <c r="B88" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
-      <c r="A88" s="1" t="s">
+    <row r="89" spans="1:12">
+      <c r="A89" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B88" s="1">
+      <c r="B89" s="1">
         <v>1</v>
       </c>
-      <c r="C88" s="2" t="s">
+      <c r="C89" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D88" s="1" t="s">
+      <c r="D89" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E88" s="1">
+      <c r="E89" s="1">
         <v>1997</v>
       </c>
-      <c r="F88" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I88" s="1" t="s">
+      <c r="F89" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I89" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J88" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K88" s="1">
+      <c r="J89" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K89" s="1">
         <v>4</v>
       </c>
-      <c r="L88" s="1" t="s">
+      <c r="L89" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
-      <c r="B89" s="1">
+    <row r="90" spans="1:12">
+      <c r="B90" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
-      <c r="A90" s="1" t="s">
+    <row r="91" spans="1:12">
+      <c r="A91" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B90" s="1">
+      <c r="B91" s="1">
         <v>1</v>
       </c>
-      <c r="C90" s="1" t="s">
+      <c r="C91" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D90" s="1" t="s">
+      <c r="D91" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E90" s="1">
+      <c r="E91" s="1">
         <v>2014</v>
-      </c>
-      <c r="F90" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G90" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H90" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I90" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J90" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K90" s="1">
-        <v>2</v>
-      </c>
-      <c r="L90" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12">
-      <c r="B91" s="1">
-        <v>2</v>
-      </c>
-      <c r="C91" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D91" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E91" s="1">
-        <v>2015</v>
       </c>
       <c r="F91" s="1" t="s">
         <v>42</v>
@@ -4503,13 +4509,13 @@
         <v>13</v>
       </c>
       <c r="I91" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J91" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K91" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L91" s="1" t="s">
         <v>31</v>
@@ -4517,54 +4523,54 @@
     </row>
     <row r="92" spans="1:12">
       <c r="B92" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="E92" s="1">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H92" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J92" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K92" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L92" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="93" spans="1:12">
       <c r="B93" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E93" s="1">
         <v>2018</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G93" s="1" t="s">
         <v>28</v>
@@ -4576,10 +4582,10 @@
         <v>14</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K93" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L93" s="1" t="s">
         <v>15</v>
@@ -4587,54 +4593,54 @@
     </row>
     <row r="94" spans="1:12">
       <c r="B94" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="E94" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H94" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I94" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K94" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L94" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="95" spans="1:12">
       <c r="B95" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E95" s="1">
         <v>2019</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G95" s="1" t="s">
         <v>13</v>
@@ -4649,7 +4655,7 @@
         <v>13</v>
       </c>
       <c r="K95" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L95" s="1" t="s">
         <v>31</v>
@@ -4657,16 +4663,16 @@
     </row>
     <row r="96" spans="1:12">
       <c r="B96" s="1">
-        <v>7</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>161</v>
+        <v>6</v>
+      </c>
+      <c r="C96" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E96" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F96" s="1" t="s">
         <v>42</v>
@@ -4684,21 +4690,21 @@
         <v>13</v>
       </c>
       <c r="K96" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L96" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="97" spans="2:12">
       <c r="B97" s="1">
-        <v>8</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E97" s="1">
         <v>2020</v>
@@ -4713,15 +4719,50 @@
         <v>13</v>
       </c>
       <c r="I97" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J97" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K97" s="1">
+        <v>2</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="98" spans="2:12">
+      <c r="B98" s="1">
+        <v>8</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E98" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F98" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I98" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J97" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K97" s="1">
+      <c r="J98" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K98" s="1">
         <v>5</v>
       </c>
-      <c r="L97" s="1" t="s">
+      <c r="L98" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add Archimedes Optimization Algorithm (ArchOA) to Physics-based group
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="726" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="734" uniqueCount="213">
   <si>
     <t>Group</t>
   </si>
@@ -652,13 +652,19 @@
   </si>
   <si>
     <t>AO</t>
+  </si>
+  <si>
+    <t>Archimedes Optimization Algorithm</t>
+  </si>
+  <si>
+    <t>ArchOA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="24">
+  <fonts count="25">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -832,6 +838,13 @@
       <b/>
       <sz val="9.8000000000000007"/>
       <color rgb="FF080808"/>
+      <name val="Fira Code"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="9.8000000000000007"/>
+      <color rgb="FF8C8C8C"/>
       <name val="Fira Code"/>
       <family val="3"/>
     </font>
@@ -1177,7 +1190,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1195,6 +1208,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1552,10 +1568,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M98"/>
+  <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="M82" sqref="M82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -3489,57 +3505,57 @@
       <c r="B57" s="1">
         <v>10</v>
       </c>
+      <c r="C57" s="7" t="s">
+        <v>211</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="E57" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F57" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H57" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I57" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J57" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K57" s="1">
+        <v>6</v>
+      </c>
+      <c r="L57" s="1" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="58" spans="1:12">
-      <c r="A58" s="1" t="s">
+      <c r="B58" s="1">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="59" spans="1:12">
+      <c r="A59" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B58" s="1">
+      <c r="B59" s="1">
         <v>1</v>
       </c>
-      <c r="C58" s="1" t="s">
+      <c r="C59" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="D58" s="1" t="s">
+      <c r="D59" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E58" s="1">
+      <c r="E59" s="1">
         <v>1994</v>
-      </c>
-      <c r="F58" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I58" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J58" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K58" s="1">
-        <v>3</v>
-      </c>
-      <c r="L58" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12">
-      <c r="B59" s="1">
-        <v>2</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>185</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="E59" s="1">
-        <v>2007</v>
       </c>
       <c r="F59" s="1" t="s">
         <v>12</v>
@@ -3554,59 +3570,59 @@
         <v>14</v>
       </c>
       <c r="J59" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K59" s="1">
-        <v>10</v>
+        <v>3</v>
       </c>
       <c r="L59" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="60" spans="1:12">
       <c r="B60" s="1">
-        <v>3</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>112</v>
+        <v>2</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>185</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>113</v>
+        <v>186</v>
       </c>
       <c r="E60" s="1">
-        <v>2011</v>
+        <v>2007</v>
       </c>
       <c r="F60" s="1" t="s">
         <v>12</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H60" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I60" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J60" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K60" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L60" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:12">
       <c r="B61" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="E61" s="1">
         <v>2011</v>
@@ -3615,39 +3631,39 @@
         <v>12</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H61" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I61" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J61" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K61" s="1">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="L61" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="62" spans="1:12">
       <c r="B62" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="E62" s="1">
-        <v>2019</v>
+        <v>2011</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G62" s="1" t="s">
         <v>13</v>
@@ -3656,36 +3672,36 @@
         <v>13</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J62" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K62" s="1">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="L62" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
     </row>
     <row r="63" spans="1:12">
       <c r="B63" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E63" s="1">
         <v>2019</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H63" s="1" t="s">
         <v>13</v>
@@ -3697,21 +3713,21 @@
         <v>28</v>
       </c>
       <c r="K63" s="1">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="L63" s="1" t="s">
-        <v>31</v>
+        <v>37</v>
       </c>
     </row>
     <row r="64" spans="1:12">
       <c r="B64" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="E64" s="1">
         <v>2019</v>
@@ -3732,21 +3748,21 @@
         <v>28</v>
       </c>
       <c r="K64" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L64" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="65" spans="1:12">
       <c r="B65" s="1">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="E65" s="1">
         <v>2019</v>
@@ -3755,13 +3771,13 @@
         <v>12</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H65" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I65" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J65" s="1" t="s">
         <v>28</v>
@@ -3775,13 +3791,13 @@
     </row>
     <row r="66" spans="1:12">
       <c r="B66" s="1">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E66" s="1">
         <v>2019</v>
@@ -3796,13 +3812,13 @@
         <v>13</v>
       </c>
       <c r="I66" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J66" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K66" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L66" s="1" t="s">
         <v>15</v>
@@ -3810,19 +3826,19 @@
     </row>
     <row r="67" spans="1:12">
       <c r="B67" s="1">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="E67" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G67" s="1" t="s">
         <v>13</v>
@@ -3831,33 +3847,33 @@
         <v>13</v>
       </c>
       <c r="I67" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J67" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K67" s="1">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="L67" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="68" spans="1:12">
       <c r="B68" s="1">
-        <v>11</v>
-      </c>
-      <c r="C68" s="3" t="s">
-        <v>172</v>
+        <v>10</v>
+      </c>
+      <c r="C68" s="1" t="s">
+        <v>126</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>173</v>
+        <v>127</v>
       </c>
       <c r="E68" s="1">
         <v>2020</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G68" s="1" t="s">
         <v>13</v>
@@ -3866,13 +3882,13 @@
         <v>13</v>
       </c>
       <c r="I68" s="1" t="s">
-        <v>63</v>
+        <v>20</v>
       </c>
       <c r="J68" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K68" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L68" s="1" t="s">
         <v>31</v>
@@ -3880,13 +3896,13 @@
     </row>
     <row r="69" spans="1:12">
       <c r="B69" s="1">
-        <v>12</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>179</v>
+        <v>11</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="E69" s="1">
         <v>2020</v>
@@ -3901,10 +3917,10 @@
         <v>13</v>
       </c>
       <c r="I69" s="1" t="s">
-        <v>20</v>
+        <v>63</v>
       </c>
       <c r="J69" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K69" s="1">
         <v>2</v>
@@ -3915,62 +3931,62 @@
     </row>
     <row r="70" spans="1:12">
       <c r="B70" s="1">
-        <v>13</v>
+        <v>12</v>
+      </c>
+      <c r="C70" s="4" t="s">
+        <v>179</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="E70" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F70" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I70" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J70" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K70" s="1">
+        <v>2</v>
+      </c>
+      <c r="L70" s="1" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="71" spans="1:12">
-      <c r="A71" s="1" t="s">
+      <c r="B71" s="1">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="72" spans="1:12">
+      <c r="A72" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B71" s="1">
+      <c r="B72" s="1">
         <v>1</v>
       </c>
-      <c r="C71" s="1" t="s">
+      <c r="C72" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="D71" s="1" t="s">
+      <c r="D72" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="E71" s="1">
+      <c r="E72" s="1">
         <v>2006</v>
       </c>
-      <c r="F71" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H71" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I71" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J71" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K71" s="1">
-        <v>5</v>
-      </c>
-      <c r="L71" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12">
-      <c r="B72" s="1">
-        <v>2</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="D72" s="1" t="s">
-        <v>132</v>
-      </c>
-      <c r="E72" s="1">
-        <v>2008</v>
-      </c>
       <c r="F72" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G72" s="1" t="s">
         <v>13</v>
@@ -3985,7 +4001,7 @@
         <v>28</v>
       </c>
       <c r="K72" s="1">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="L72" s="1" t="s">
         <v>15</v>
@@ -3993,51 +4009,51 @@
     </row>
     <row r="73" spans="1:12">
       <c r="B73" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E73" s="1">
-        <v>2016</v>
+        <v>2008</v>
       </c>
       <c r="F73" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H73" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I73" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J73" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K73" s="1">
         <v>4</v>
       </c>
       <c r="L73" s="1" t="s">
-        <v>49</v>
+        <v>15</v>
       </c>
     </row>
     <row r="74" spans="1:12">
       <c r="B74" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E74" s="1">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="F74" s="1" t="s">
         <v>42</v>
@@ -4049,36 +4065,36 @@
         <v>13</v>
       </c>
       <c r="I74" s="1" t="s">
-        <v>14</v>
+        <v>63</v>
       </c>
       <c r="J74" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K74" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L74" s="1" t="s">
-        <v>15</v>
+        <v>49</v>
       </c>
     </row>
     <row r="75" spans="1:12">
       <c r="B75" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>70</v>
+        <v>137</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>71</v>
+        <v>138</v>
       </c>
       <c r="E75" s="1">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F75" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H75" s="1" t="s">
         <v>13</v>
@@ -4090,24 +4106,24 @@
         <v>28</v>
       </c>
       <c r="K75" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="L75" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="76" spans="1:12">
       <c r="B76" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>139</v>
+        <v>70</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>140</v>
+        <v>71</v>
       </c>
       <c r="E76" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F76" s="1" t="s">
         <v>42</v>
@@ -4125,7 +4141,7 @@
         <v>28</v>
       </c>
       <c r="K76" s="1">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="L76" s="1" t="s">
         <v>31</v>
@@ -4133,22 +4149,22 @@
     </row>
     <row r="77" spans="1:12">
       <c r="B77" s="1">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>157</v>
+        <v>139</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>158</v>
+        <v>140</v>
       </c>
       <c r="E77" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F77" s="1" t="s">
         <v>42</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H77" s="1" t="s">
         <v>13</v>
@@ -4160,73 +4176,73 @@
         <v>28</v>
       </c>
       <c r="K77" s="1">
-        <v>3</v>
+        <v>12</v>
       </c>
       <c r="L77" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="78" spans="1:12">
       <c r="B78" s="1">
+        <v>7</v>
+      </c>
+      <c r="C78" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="E78" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F78" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H78" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I78" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J78" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K78" s="1">
+        <v>3</v>
+      </c>
+      <c r="L78" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="79" spans="1:12">
+      <c r="B79" s="1">
         <v>8</v>
       </c>
     </row>
-    <row r="79" spans="1:12">
-      <c r="A79" s="1" t="s">
+    <row r="80" spans="1:12">
+      <c r="A80" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B79" s="1">
+      <c r="B80" s="1">
         <v>1</v>
       </c>
-      <c r="C79" s="1" t="s">
+      <c r="C80" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="D79" s="1" t="s">
+      <c r="D80" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E79" s="1">
+      <c r="E80" s="1">
         <v>2018</v>
       </c>
-      <c r="F79" s="1" t="s">
+      <c r="F80" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G79" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H79" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I79" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J79" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K79" s="1">
-        <v>4</v>
-      </c>
-      <c r="L79" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12">
-      <c r="B80" s="1">
-        <v>2</v>
-      </c>
-      <c r="C80" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="D80" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="E80" s="1">
-        <v>2012</v>
-      </c>
-      <c r="F80" s="1" t="s">
-        <v>12</v>
-      </c>
       <c r="G80" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H80" s="1" t="s">
         <v>13</v>
@@ -4238,7 +4254,7 @@
         <v>28</v>
       </c>
       <c r="K80" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="L80" s="1" t="s">
         <v>31</v>
@@ -4246,112 +4262,112 @@
     </row>
     <row r="81" spans="1:12">
       <c r="B81" s="1">
-        <v>3</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>146</v>
+        <v>2</v>
+      </c>
+      <c r="C81" s="4" t="s">
+        <v>183</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>147</v>
+        <v>184</v>
       </c>
       <c r="E81" s="1">
-        <v>2019</v>
+        <v>2012</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H81" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I81" s="1" t="s">
-        <v>63</v>
+        <v>14</v>
       </c>
       <c r="J81" s="1" t="s">
         <v>28</v>
       </c>
       <c r="K81" s="1">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="L81" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="82" spans="1:12">
       <c r="B82" s="1">
+        <v>3</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="E82" s="1">
+        <v>2019</v>
+      </c>
+      <c r="F82" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H82" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I82" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="J82" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K82" s="1">
+        <v>2</v>
+      </c>
+      <c r="L82" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="83" spans="1:12">
+      <c r="B83" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="83" spans="1:12">
-      <c r="A83" s="1" t="s">
+    <row r="84" spans="1:12">
+      <c r="A84" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B83" s="1">
+      <c r="B84" s="1">
         <v>1</v>
       </c>
-      <c r="C83" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>189</v>
       </c>
-      <c r="D83" s="1" t="s">
+      <c r="D84" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E83" s="1">
+      <c r="E84" s="1">
         <v>1993</v>
       </c>
-      <c r="F83" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I83" s="1" t="s">
+      <c r="F84" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I84" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="J83" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K83" s="1">
+      <c r="J84" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K84" s="1">
         <v>3</v>
-      </c>
-      <c r="L83" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12">
-      <c r="B84" s="1">
-        <v>2</v>
-      </c>
-      <c r="C84" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="E84" s="1">
-        <v>2016</v>
-      </c>
-      <c r="F84" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G84" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I84" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J84" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K84" s="1">
-        <v>2</v>
       </c>
       <c r="L84" s="1" t="s">
         <v>15</v>
@@ -4359,22 +4375,22 @@
     </row>
     <row r="85" spans="1:12">
       <c r="B85" s="1">
-        <v>3</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>207</v>
+        <v>2</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>149</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>208</v>
+        <v>150</v>
       </c>
       <c r="E85" s="1">
-        <v>2021</v>
+        <v>2016</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H85" s="1" t="s">
         <v>13</v>
@@ -4383,10 +4399,10 @@
         <v>14</v>
       </c>
       <c r="J85" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K85" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L85" s="1" t="s">
         <v>15</v>
@@ -4394,145 +4410,145 @@
     </row>
     <row r="86" spans="1:12">
       <c r="B86" s="1">
+        <v>3</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>207</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="E86" s="1">
+        <v>2021</v>
+      </c>
+      <c r="F86" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H86" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I86" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="J86" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K86" s="1">
+        <v>6</v>
+      </c>
+      <c r="L86" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12">
+      <c r="B87" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:12">
-      <c r="A87" s="1" t="s">
+    <row r="88" spans="1:12">
+      <c r="A88" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="B87" s="1">
+      <c r="B88" s="1">
         <v>1</v>
       </c>
-      <c r="C87" s="1" t="s">
+      <c r="C88" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="D87" s="1" t="s">
+      <c r="D88" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="E87" s="1">
+      <c r="E88" s="1">
         <v>2001</v>
       </c>
-      <c r="F87" s="1" t="s">
+      <c r="F88" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G87" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="H87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I87" s="1" t="s">
+      <c r="G88" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="H88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I88" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J87" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K87" s="1">
+      <c r="J88" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K88" s="1">
         <v>5</v>
       </c>
-      <c r="L87" s="1" t="s">
+      <c r="L88" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="88" spans="1:12">
-      <c r="B88" s="1">
+    <row r="89" spans="1:12">
+      <c r="B89" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="89" spans="1:12">
-      <c r="A89" s="1" t="s">
+    <row r="90" spans="1:12">
+      <c r="A90" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="B89" s="1">
+      <c r="B90" s="1">
         <v>1</v>
       </c>
-      <c r="C89" s="2" t="s">
+      <c r="C90" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D89" s="1" t="s">
+      <c r="D90" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="E89" s="1">
+      <c r="E90" s="1">
         <v>1997</v>
       </c>
-      <c r="F89" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="G89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I89" s="1" t="s">
+      <c r="F90" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I90" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J89" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K89" s="1">
+      <c r="J90" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K90" s="1">
         <v>4</v>
       </c>
-      <c r="L89" s="1" t="s">
+      <c r="L90" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="90" spans="1:12">
-      <c r="B90" s="1">
+    <row r="91" spans="1:12">
+      <c r="B91" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="91" spans="1:12">
-      <c r="A91" s="1" t="s">
+    <row r="92" spans="1:12">
+      <c r="A92" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="B91" s="1">
+      <c r="B92" s="1">
         <v>1</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C92" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D91" s="1" t="s">
+      <c r="D92" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E91" s="1">
+      <c r="E92" s="1">
         <v>2014</v>
-      </c>
-      <c r="F91" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="G91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="H91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="I91" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J91" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="K91" s="1">
-        <v>2</v>
-      </c>
-      <c r="L91" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12">
-      <c r="B92" s="1">
-        <v>2</v>
-      </c>
-      <c r="C92" s="1" t="s">
-        <v>133</v>
-      </c>
-      <c r="D92" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="E92" s="1">
-        <v>2015</v>
       </c>
       <c r="F92" s="1" t="s">
         <v>42</v>
@@ -4544,13 +4560,13 @@
         <v>13</v>
       </c>
       <c r="I92" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J92" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K92" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="L92" s="1" t="s">
         <v>31</v>
@@ -4558,54 +4574,54 @@
     </row>
     <row r="93" spans="1:12">
       <c r="B93" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>74</v>
+        <v>133</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>75</v>
+        <v>134</v>
       </c>
       <c r="E93" s="1">
-        <v>2018</v>
+        <v>2015</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="H93" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I93" s="1" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="J93" s="1" t="s">
-        <v>28</v>
+        <v>13</v>
       </c>
       <c r="K93" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L93" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="94" spans="1:12">
       <c r="B94" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E94" s="1">
         <v>2018</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G94" s="1" t="s">
         <v>28</v>
@@ -4617,10 +4633,10 @@
         <v>14</v>
       </c>
       <c r="J94" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="K94" s="1">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="L94" s="1" t="s">
         <v>15</v>
@@ -4628,54 +4644,54 @@
     </row>
     <row r="95" spans="1:12">
       <c r="B95" s="1">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>164</v>
+        <v>76</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>163</v>
+        <v>77</v>
       </c>
       <c r="E95" s="1">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="H95" s="1" t="s">
         <v>13</v>
       </c>
       <c r="I95" s="1" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="J95" s="1" t="s">
         <v>13</v>
       </c>
       <c r="K95" s="1">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="L95" s="1" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
     </row>
     <row r="96" spans="1:12">
       <c r="B96" s="1">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>159</v>
+        <v>164</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="E96" s="1">
         <v>2019</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="G96" s="1" t="s">
         <v>13</v>
@@ -4690,7 +4706,7 @@
         <v>13</v>
       </c>
       <c r="K96" s="1">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L96" s="1" t="s">
         <v>31</v>
@@ -4698,16 +4714,16 @@
     </row>
     <row r="97" spans="2:12">
       <c r="B97" s="1">
-        <v>7</v>
-      </c>
-      <c r="C97" s="2" t="s">
-        <v>161</v>
+        <v>6</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>159</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="E97" s="1">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="F97" s="1" t="s">
         <v>42</v>
@@ -4725,21 +4741,21 @@
         <v>13</v>
       </c>
       <c r="K97" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="L97" s="1" t="s">
-        <v>15</v>
+        <v>31</v>
       </c>
     </row>
     <row r="98" spans="2:12">
       <c r="B98" s="1">
-        <v>8</v>
-      </c>
-      <c r="C98" s="1" t="s">
-        <v>141</v>
+        <v>7</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>161</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="E98" s="1">
         <v>2020</v>
@@ -4754,15 +4770,50 @@
         <v>13</v>
       </c>
       <c r="I98" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="J98" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K98" s="1">
+        <v>2</v>
+      </c>
+      <c r="L98" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="99" spans="2:12">
+      <c r="B99" s="1">
+        <v>8</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="E99" s="1">
+        <v>2020</v>
+      </c>
+      <c r="F99" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="G99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H99" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="I99" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="J98" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="K98" s="1">
+      <c r="J99" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="K99" s="1">
         <v>5</v>
       </c>
-      <c r="L98" s="1" t="s">
+      <c r="L99" s="1" t="s">
         <v>31</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update ref for ArchOA algorithm
</commit_message>
<xml_diff>
--- a/models_history.xlsx
+++ b/models_history.xlsx
@@ -1570,8 +1570,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="M82" sqref="M82"/>
+    <sheetView tabSelected="1" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6"/>
@@ -3512,7 +3512,7 @@
         <v>212</v>
       </c>
       <c r="E57" s="1">
-        <v>2020</v>
+        <v>2021</v>
       </c>
       <c r="F57" s="1" t="s">
         <v>12</v>

</xml_diff>